<commit_message>
Actualizado el diagrama con una nueva hoja
Esta hoja solo contiene las horas divididas por semana
</commit_message>
<xml_diff>
--- a/Documentos/Sprint2(1).xlsx
+++ b/Documentos/Sprint2(1).xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2 - Grupo" sheetId="1" r:id="rId1"/>
-    <sheet name="Reuniones" sheetId="2" r:id="rId2"/>
+    <sheet name="Horas Por Semanas" sheetId="3" r:id="rId2"/>
+    <sheet name="Reuniones" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="66">
   <si>
     <t>Elemento</t>
   </si>
@@ -6879,6 +6880,54 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B1:D11" totalsRowShown="0">
+  <autoFilter ref="B1:D11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nombre"/>
+    <tableColumn id="2" name="Trabajos Designados"/>
+    <tableColumn id="3" name="Horas Totales _x000a_Asignadas por Tarea"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="B14:D21" totalsRowShown="0">
+  <autoFilter ref="B14:D21"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nombre"/>
+    <tableColumn id="2" name="Trabajos Designados"/>
+    <tableColumn id="3" name="Horas Totales _x000a_Asignadas por Tarea"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="B25:D35" totalsRowShown="0">
+  <autoFilter ref="B25:D35"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nombre"/>
+    <tableColumn id="2" name="Trabajos Designados"/>
+    <tableColumn id="3" name="Horas Totales _x000a_Asignadas por Tarea"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="B39:D44" totalsRowShown="0">
+  <autoFilter ref="B39:D44"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nombre"/>
+    <tableColumn id="2" name="Trabajos Designados"/>
+    <tableColumn id="3" name="Horas Totales _x000a_Asignadas por Tarea"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -7079,8 +7128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C47"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -9401,6 +9450,393 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="24.875" customWidth="1"/>
+    <col min="4" max="4" width="37.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1009"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>